<commit_message>
ft slides and UML diagrams
</commit_message>
<xml_diff>
--- a/project/phase-n-time-sheet.xlsx
+++ b/project/phase-n-time-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timwood/Google Drive/courses/distrib-sys/20-dist-sys/gwDistSys20.github.io/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{492EAB2D-8866-3946-BD6E-991D2B0A856D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91ED206-0A0B-6449-9503-8104734FF0D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="460" windowWidth="50060" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="460" windowWidth="19580" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time sheet" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
-  <si>
-    <t>Phase n</t>
-  </si>
   <si>
     <t>Group Name</t>
   </si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>FILL IN</t>
+  </si>
+  <si>
+    <t>Report # FILL IN</t>
   </si>
 </sst>
 </file>
@@ -1566,7 +1566,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1605,7 +1605,7 @@
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
       <c r="A3" s="46"/>
       <c r="B3" s="47" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C3" s="48"/>
       <c r="D3" s="48"/>
@@ -1627,7 +1627,7 @@
     <row r="5" spans="1:8" ht="48" customHeight="1">
       <c r="A5" s="54"/>
       <c r="B5" s="55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="56"/>
       <c r="D5" s="56"/>
@@ -1649,11 +1649,11 @@
     <row r="7" spans="1:8" ht="18" customHeight="1">
       <c r="A7" s="59"/>
       <c r="B7" s="61" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="35"/>
       <c r="D7" s="61" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" s="35"/>
       <c r="F7" s="35"/>
@@ -1662,11 +1662,11 @@
     <row r="8" spans="1:8" ht="18" customHeight="1">
       <c r="A8" s="53"/>
       <c r="B8" s="63" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="36"/>
       <c r="D8" s="64" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" s="35"/>
       <c r="F8" s="35"/>
@@ -1685,11 +1685,11 @@
     <row r="10" spans="1:8" ht="16">
       <c r="A10" s="51"/>
       <c r="B10" s="61" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="35"/>
       <c r="D10" s="61" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" s="35"/>
       <c r="F10" s="35"/>
@@ -1699,7 +1699,7 @@
     <row r="11" spans="1:8" ht="16">
       <c r="A11" s="51"/>
       <c r="B11" s="67" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="67"/>
       <c r="D11" s="68">
@@ -1734,26 +1734,26 @@
       <c r="A14" s="72"/>
       <c r="B14" s="80"/>
       <c r="C14" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="81" t="s">
+      <c r="E14" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="81" t="s">
+      <c r="F14" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="81" t="s">
+      <c r="G14" s="81" t="s">
         <v>9</v>
-      </c>
-      <c r="G14" s="81" t="s">
-        <v>10</v>
       </c>
       <c r="H14" s="72"/>
     </row>
     <row r="15" spans="1:8" ht="21" customHeight="1">
       <c r="A15" s="53"/>
       <c r="B15" s="82" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="83">
         <v>25</v>
@@ -1776,7 +1776,7 @@
     <row r="16" spans="1:8" ht="21" customHeight="1">
       <c r="A16" s="53"/>
       <c r="B16" s="82" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="83"/>
       <c r="D16" s="83">
@@ -1797,7 +1797,7 @@
     <row r="17" spans="1:8" ht="21" customHeight="1">
       <c r="A17" s="53"/>
       <c r="B17" s="82" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="83">
         <v>40</v>
@@ -1820,7 +1820,7 @@
     <row r="18" spans="1:8" ht="21" customHeight="1">
       <c r="A18" s="53"/>
       <c r="B18" s="82" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="83">
         <v>30</v>
@@ -1853,7 +1853,7 @@
     <row r="20" spans="1:8" ht="21" customHeight="1">
       <c r="A20" s="73"/>
       <c r="B20" s="87" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="88">
         <f t="shared" ref="C20:G20" si="1">SUM(C15:C19)</f>
@@ -1968,11 +1968,11 @@
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
       <c r="A3" s="5"/>
       <c r="B3" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="32"/>
       <c r="D3" s="33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="32"/>
       <c r="F3" s="32"/>
@@ -1992,7 +1992,7 @@
     <row r="5" spans="1:8" ht="30.75" customHeight="1">
       <c r="A5" s="7"/>
       <c r="B5" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -2216,7 +2216,7 @@
     <row r="25" spans="1:8" ht="30" customHeight="1">
       <c r="A25" s="7"/>
       <c r="B25" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>

</xml_diff>